<commit_message>
cap nhat import vat tu
</commit_message>
<xml_diff>
--- a/frontend/importVatTu.xlsx
+++ b/frontend/importVatTu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LEARNING\project\kimhung\kimhung\frontend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LEARNING\project\kimhung\Source\kimhung\frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037F1CC7-D900-4690-B4FD-6A515CF2B625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4127FE-59D9-4C89-A848-29F77ECDB47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>MaVatTu</t>
   </si>
@@ -42,56 +42,59 @@
     <t>GiaBan</t>
   </si>
   <si>
-    <t>bl6x60</t>
-  </si>
-  <si>
-    <t>bulon RS 6 x 60(1.000 con/bao)</t>
-  </si>
-  <si>
-    <t>con</t>
-  </si>
-  <si>
-    <t>u8x114</t>
-  </si>
-  <si>
-    <t>cùm u 8 x 114</t>
-  </si>
-  <si>
     <t>bộ</t>
   </si>
   <si>
-    <t>ld6x33d</t>
-  </si>
-  <si>
-    <t>long đền 6x33 dày</t>
-  </si>
-  <si>
-    <t>blk16x280</t>
-  </si>
-  <si>
-    <t>bulon NR thân nhỏ 16x280</t>
-  </si>
-  <si>
-    <t>rct30</t>
-  </si>
-  <si>
-    <t>răng cây thép 30 x 1m</t>
-  </si>
-  <si>
-    <t>cây</t>
-  </si>
-  <si>
-    <t>M</t>
+    <t>I</t>
+  </si>
+  <si>
+    <t>bulon 6x60 (inox 304)</t>
+  </si>
+  <si>
+    <t>bulon 6x70 (inox 304)</t>
+  </si>
+  <si>
+    <t>bulon 6x80 (inox 304)</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>bl6x60-i304-test1</t>
+  </si>
+  <si>
+    <t>bl6x70-i304-test2</t>
+  </si>
+  <si>
+    <t>bl6x80-i304-test3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -113,14 +116,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,114 +425,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="E2" s="4">
+        <v>1510</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <v>3631</v>
+        <v>5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1690</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5">
-        <v>7100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6">
-        <v>103000</v>
+        <v>5</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1860</v>
       </c>
     </row>
   </sheetData>

</xml_diff>